<commit_message>
Imported the data set and created the mortality tables
</commit_message>
<xml_diff>
--- a/CMI Mort Data.xlsx
+++ b/CMI Mort Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitypretoria-my.sharepoint.com/personal/u21626562_up_ac_za/Documents/UP/Modules/Honours/NPN 780/Methodology/R project/Main Research Project GitHub Repo/longevity-bonds-project2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{01EF1DC0-8117-473A-97FA-2989928FA2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6968B70-48BC-44D2-85DD-22CC4BED086E}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{01EF1DC0-8117-473A-97FA-2989928FA2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD21A8E5-D0AC-47E6-AB7C-98914AD775A4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{AE1D289B-61BA-4089-BBBA-B2AE61AC16C6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{AE1D289B-61BA-4089-BBBA-B2AE61AC16C6}"/>
   </bookViews>
   <sheets>
     <sheet name="M L Exposure" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5652B66C-31A4-4BC6-8FDF-748BBE3E6122}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +1997,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A48" sqref="A48:L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -3366,30 +3366,14 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="6"/>
-      <c r="B48" s="7">
-        <v>163</v>
-      </c>
-      <c r="C48" s="8">
-        <v>211</v>
-      </c>
-      <c r="D48" s="8">
-        <v>265</v>
-      </c>
-      <c r="E48" s="8">
-        <v>248</v>
-      </c>
-      <c r="F48" s="8">
-        <v>144</v>
-      </c>
-      <c r="G48" s="8">
-        <v>123</v>
-      </c>
-      <c r="H48" s="8">
-        <v>70</v>
-      </c>
-      <c r="I48" s="8">
-        <v>26</v>
-      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
@@ -3403,7 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9B5BB1-CB84-4C41-B19C-0FF7C792E405}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4730,7 +4714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEEF6465-FF0F-436F-93D8-DCAB4D35D6C0}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -18884,7 +18868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE170AA-F21B-4A49-9A35-E0CC98D8B84A}">
   <dimension ref="A1:AR96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>